<commit_message>
docs: update Product Backlog and User Stories with accurate points for Sprint tracking
</commit_message>
<xml_diff>
--- a/Product Documents/User_Stories.xlsx
+++ b/Product Documents/User_Stories.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="3W4ERGsCx9QuF2dpqWj4bDZKPd1LTeRxevtiGozOrYI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="6IMqqrlblR+VuCMmO0bequI4Vwqqwl7YFwd31zraW+s="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
@@ -78,6 +78,9 @@
     <t>As a Customer, I want to browse and filter menu items so that I can choose meals that fit my needs</t>
   </si>
   <si>
+    <t>Medium</t>
+  </si>
+  <si>
     <t>Payment Processing</t>
   </si>
   <si>
@@ -102,6 +105,9 @@
     <t>As a Customer, I want to leave a rating and write a review so that I can share my experience with others.</t>
   </si>
   <si>
+    <t>Low</t>
+  </si>
+  <si>
     <t>Promotional Code Generator</t>
   </si>
   <si>
@@ -114,7 +120,16 @@
     <t>As a Customer, I want to enter a promo code at checkout so that I can receive discounts on my order.</t>
   </si>
   <si>
-    <t>Low</t>
+    <t>Order Tracking</t>
+  </si>
+  <si>
+    <t>track the status of my order</t>
+  </si>
+  <si>
+    <t>I can see when my order will be ready</t>
+  </si>
+  <si>
+    <t>As a Customer, I want to track the status of my order so I can see when my order will be ready</t>
   </si>
   <si>
     <t>Collect and Use Data of Orders Over Time</t>
@@ -130,9 +145,6 @@
   </si>
   <si>
     <t>As a Manager, I want to analyze order trends over time so that I can make data-informed business decisions.</t>
-  </si>
-  <si>
-    <t>Medium</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -142,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -191,11 +203,6 @@
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color rgb="FF2D3B45"/>
-      <name val="Consolas"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -247,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border/>
     <border>
       <left/>
@@ -346,20 +353,6 @@
       </bottom>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFC7CDD1"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFC7CDD1"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFC7CDD1"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFC7CDD1"/>
-      </bottom>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFBFBFBF"/>
       </left>
@@ -382,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -427,21 +420,24 @@
     <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="8" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf borderId="10" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -451,12 +447,12 @@
     <xf borderId="10" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="6" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="12" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -781,10 +777,10 @@
         <v>19</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="18">
-        <v>3.0</v>
+        <v>20</v>
+      </c>
+      <c r="H5" s="16">
+        <v>5.0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -792,25 +788,25 @@
         <v>3.0</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H6" s="16">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -818,22 +814,22 @@
         <v>4.0</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="H7" s="16">
         <v>3.0</v>
@@ -844,164 +840,189 @@
         <v>5.0</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H8" s="16">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="10">
+      <c r="A9" s="19">
         <v>6.0</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="13" t="s">
         <v>36</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="H9" s="16">
-        <v>13.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="18">
-        <v>0.0</v>
+      <c r="A10" s="19">
+        <v>7.0</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="16">
+        <v>8.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="18">
+      <c r="H11" s="23">
         <v>0.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="18">
+      <c r="H12" s="23">
         <v>0.0</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="10"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="18">
+      <c r="H13" s="23">
         <v>0.0</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="10"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="18">
+      <c r="H14" s="23">
         <v>0.0</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="10"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="15"/>
-      <c r="H15" s="18">
+      <c r="H15" s="23">
         <v>0.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="10"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="18">
+      <c r="H16" s="23">
         <v>0.0</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="10"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="18">
+      <c r="H17" s="23">
         <v>0.0</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29">
-        <f>SUM(H4:H17)</f>
-        <v>32</v>
+      <c r="A18" s="10"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="23">
+        <v>0.0</v>
       </c>
     </row>
-    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30">
+        <f>SUM(H4:H18)</f>
+        <v>42</v>
+      </c>
+    </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -1983,14 +2004,15 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A19:G19"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G17">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G18">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>